<commit_message>
- update code to support mobile web testing via browserstack.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-05.data.xlsx
+++ b/artifact/data/web-05.data.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0182D7-D7FB-6E44-8F8E-471ED1CA4B66}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3DAB8D-0389-2C4B-BF62-9D0A12016864}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="34600" windowHeight="17620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="locators-xpath" sheetId="8" r:id="rId2"/>
+    <sheet name="locators-xpath-android" sheetId="10" r:id="rId3"/>
+    <sheet name="locators-xpath-iphone" sheetId="11" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
   <si>
     <t>true</t>
   </si>
@@ -299,6 +301,42 @@
   </si>
   <si>
     <t>browserstack</t>
+  </si>
+  <si>
+    <t>browserstack.local</t>
+  </si>
+  <si>
+    <t>ANDROID</t>
+  </si>
+  <si>
+    <t>browserstack.os</t>
+  </si>
+  <si>
+    <t>browserstack.os_version</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>browserstack.device</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S8</t>
+  </si>
+  <si>
+    <t>browserstack.real_mobile</t>
+  </si>
+  <si>
+    <t>browserstack.debug</t>
+  </si>
+  <si>
+    <t>IOS</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>iPhone X</t>
   </si>
 </sst>
 </file>
@@ -427,7 +465,341 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1170,40 +1542,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="22" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="48" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="47" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="19" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="17" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="43" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="42" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1216,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
   <dimension ref="A1:AAA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="192" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A9" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1540,6 +1912,752 @@
     <sortCondition ref="A1:A25"/>
   </sortState>
   <conditionalFormatting sqref="A15:A1048576">
+    <cfRule type="beginsWith" dxfId="38" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="37" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="36" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B1048576 B13:B14">
+    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="34" priority="13">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A13">
+    <cfRule type="beginsWith" dxfId="33" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="32" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="31" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B13">
+    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="29" priority="8">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="beginsWith" dxfId="28" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="27" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="26" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362E671B-3266-D74C-A30E-0914D60258CD}">
+  <dimension ref="A1:AAA35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="103.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A15:A1048576">
+    <cfRule type="beginsWith" dxfId="25" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="24" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="23" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(A15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:B14 B16:B1048576">
+    <cfRule type="expression" dxfId="22" priority="12" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="21" priority="13">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A13">
+    <cfRule type="beginsWith" dxfId="20" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="19" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="18" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B13">
+    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="16" priority="8">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="beginsWith" dxfId="15" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="13" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57C66B0-9463-6444-930B-B99E0CDBA23F}">
+  <dimension ref="A1:AAA35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B35" sqref="A29:B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="103.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A15:A1048576">
     <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
@@ -1550,7 +2668,7 @@
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:B1048576 B13:B14">
+  <conditionalFormatting sqref="B13:B14 B16:B1048576">
     <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>

</xml_diff>

<commit_message>
[base] - code fix: consider "null=null" and "empty=empty" when comparing arrays
[json]
- [`assertValues(json,jsonpath,array,exactOrder)`](../commands/json/assertValues(json,jsonpath,array,exactOrder)): code
  fix to properly consider null values.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-05.data.xlsx
+++ b/artifact/data/web-05.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3DAB8D-0389-2C4B-BF62-9D0A12016864}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C149C2-1327-D149-B627-8504B6D7FB96}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -343,7 +343,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -389,6 +389,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -431,7 +437,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -452,6 +458,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1588,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
   <dimension ref="A1:AAA36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1849,8 +1859,8 @@
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>2</v>
+      <c r="B29" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1969,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362E671B-3266-D74C-A30E-0914D60258CD}">
   <dimension ref="A1:AAA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2285,51 +2295,51 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="25" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="25" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="24" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B14 B16:B1048576">
-    <cfRule type="expression" dxfId="22" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="15">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="20" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="20" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="19" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="16" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="15" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="15" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="14" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2343,7 +2353,7 @@
   <dimension ref="A1:AAA35"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B35" sqref="A29:B35"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2658,51 +2668,51 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="12" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="11" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B14 B16:B1048576">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="15">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="7" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="6" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update example data files
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-05.data.xlsx
+++ b/artifact/data/web-05.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C149C2-1327-D149-B627-8504B6D7FB96}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDCB93E-8FF2-BB40-AF7C-A42D79303009}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29000" yWindow="440" windowWidth="22200" windowHeight="17260" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="93">
   <si>
     <t>true</t>
   </si>
@@ -252,12 +252,6 @@
     <t>nexial.browser</t>
   </si>
   <si>
-    <t>nexial.browserstack.username</t>
-  </si>
-  <si>
-    <t>nexial.browserstack.automatekey</t>
-  </si>
-  <si>
     <t>nexial.browserstack.enablelocal</t>
   </si>
   <si>
@@ -291,15 +285,9 @@
     <t>8</t>
   </si>
   <si>
-    <t>crypt:b4b1e892023a8af508a8d3d5a58559b019156556e02685843ffb1e0e64f4ae11</t>
-  </si>
-  <si>
     <t>browserstack.use_w3c</t>
   </si>
   <si>
-    <t>crypt:a83bd52131dfd84aa6d410ab8dfd5956262855ad37c317be</t>
-  </si>
-  <si>
     <t>browserstack</t>
   </si>
   <si>
@@ -337,6 +325,12 @@
   </si>
   <si>
     <t>iPhone X</t>
+  </si>
+  <si>
+    <t>DON'T FORGET TO ADD 'nexial.browserstack.username' AND 'nexial.browserstack.automatekey' TO DATASHEET OR JAVA_OPT</t>
+  </si>
+  <si>
+    <t>// NOTE !!!!</t>
   </si>
 </sst>
 </file>
@@ -475,7 +469,137 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1552,40 +1676,40 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1 A3:A9 A22:A1048576">
-    <cfRule type="beginsWith" dxfId="48" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="58" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="47" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="57" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="46" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B3:B9 B22:B1048576">
-    <cfRule type="expression" dxfId="45" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="44" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="beginsWith" dxfId="43" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="53" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="52" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="39" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="5">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1596,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938A5DF5-858F-F04F-A650-D78F3893CC59}">
-  <dimension ref="A1:AAA36"/>
+  <dimension ref="A1:AAA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1836,15 +1960,15 @@
         <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>81</v>
+      <c r="B27" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1852,68 +1976,60 @@
         <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1921,53 +2037,72 @@
   <sortState ref="A1:B25">
     <sortCondition ref="A1:A25"/>
   </sortState>
-  <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="38" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <conditionalFormatting sqref="A15:A34 A36:A1048576">
+    <cfRule type="beginsWith" dxfId="48" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="37" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="47" priority="15" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="36" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:B1048576 B13:B14">
-    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
+  <conditionalFormatting sqref="B13:B14 B16:B34 B36:B1048576">
+    <cfRule type="expression" dxfId="45" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="34" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="18">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="33" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="43" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="32" priority="5" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="42" priority="10" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="31" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="29" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="13">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="28" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="38" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="37" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A35,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A35,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(B35))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1977,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362E671B-3266-D74C-A30E-0914D60258CD}">
-  <dimension ref="A1:AAA35"/>
+  <dimension ref="A1:AAA34"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2217,55 +2352,55 @@
         <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2273,74 +2408,85 @@
         <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="25" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+  <conditionalFormatting sqref="A15:A33 A35:A1048576">
+    <cfRule type="beginsWith" dxfId="35" priority="16" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="34" priority="17" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B14 B16:B1048576">
-    <cfRule type="expression" dxfId="22" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="B13:B14 B16:B33 B35:B1048576">
+    <cfRule type="expression" dxfId="32" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="20">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="20" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="30" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="29" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="16" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="15">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="15" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="25" priority="8" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="24" priority="9" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A34,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A34,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A34))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+      <formula>LEN(TRIM(B34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2350,10 +2496,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57C66B0-9463-6444-930B-B99E0CDBA23F}">
-  <dimension ref="A1:AAA35"/>
+  <dimension ref="A1:AAA34"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -2590,55 +2736,55 @@
         <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2646,73 +2792,65 @@
         <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A15:A1048576">
-    <cfRule type="beginsWith" dxfId="12" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="22" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A15,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="21" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A15,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A15))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B14 B16:B1048576">
-    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="15">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A13">
-    <cfRule type="beginsWith" dxfId="7" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="17" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="16" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B13">
-    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="12" priority="3" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="11" priority="4" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(A14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>